<commit_message>
frontend + backend changes
</commit_message>
<xml_diff>
--- a/FRONTEND/public/templates/Employee_Campaign_Assignment_Template.xlsx
+++ b/FRONTEND/public/templates/Employee_Campaign_Assignment_Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA260150-632B-4D07-99E4-A36CF5C85A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1D10FB-A8C7-4971-B1EB-0D9E40E6D761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>